<commit_message>
Continue w/ proof Sect 4, Run 1
</commit_message>
<xml_diff>
--- a/Calcs/tables.xlsx
+++ b/Calcs/tables.xlsx
@@ -14,7 +14,8 @@
   <sheets>
     <sheet name="2.1" sheetId="1" r:id="rId1"/>
     <sheet name="2.2" sheetId="2" r:id="rId2"/>
-    <sheet name="5.1" sheetId="3" r:id="rId3"/>
+    <sheet name="4.1" sheetId="4" r:id="rId3"/>
+    <sheet name="5.1" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="106">
   <si>
     <t>$$</t>
   </si>
@@ -290,6 +291,60 @@
   </si>
   <si>
     <t>\ref{x}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run </t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>1A</t>
+  </si>
+  <si>
+    <t>1B</t>
+  </si>
+  <si>
+    <t>2A</t>
+  </si>
+  <si>
+    <t>2B</t>
+  </si>
+  <si>
+    <t>2C</t>
+  </si>
+  <si>
+    <t>Fixed ends, uniform p</t>
+  </si>
+  <si>
+    <t>Simply supported ends, uniform p</t>
+  </si>
+  <si>
+    <t>Fixed ends, Capstan p z=24.5, various \mu</t>
+  </si>
+  <si>
+    <t>Simply supported ends, Capstan p z=24.5 various \mu</t>
+  </si>
+  <si>
+    <t>Focus</t>
+  </si>
+  <si>
+    <t>Barrell Stress</t>
+  </si>
+  <si>
+    <t>Barrell Buckling</t>
+  </si>
+  <si>
+    <t>Flange Stress</t>
+  </si>
+  <si>
+    <t>2D</t>
+  </si>
+  <si>
+    <t>Fixed ends, Capstan p z=0, various \mu</t>
+  </si>
+  <si>
+    <t>Simply supported ends, Capstan p z=0 various \mu</t>
   </si>
 </sst>
 </file>
@@ -379,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -414,12 +469,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -427,9 +476,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -443,20 +489,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -787,14 +845,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="12" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="12"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -981,15 +1039,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="17" t="s">
+      <c r="A1" s="15"/>
+      <c r="B1" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="16"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="14"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="13" t="s">
         <v>49</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -1010,7 +1068,7 @@
         <f>C3*25.4</f>
         <v>43.18</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="12">
         <v>1.7</v>
       </c>
       <c r="D3" s="2">
@@ -1025,7 +1083,7 @@
         <f>C4*25.4</f>
         <v>23.367999999999999</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="12">
         <v>0.92</v>
       </c>
       <c r="D4" s="2">
@@ -1040,7 +1098,7 @@
         <f>C5*25.4</f>
         <v>36.575999999999993</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="12">
         <v>1.44</v>
       </c>
       <c r="D5" s="2">
@@ -1055,7 +1113,7 @@
         <f>C6*25.4</f>
         <v>27.94</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="12">
         <v>1.1000000000000001</v>
       </c>
       <c r="D6" s="2">
@@ -1087,43 +1145,163 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="49" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>3</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>4</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="21" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="25" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="26" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" style="21" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="22"/>
+    <col min="1" max="1" width="12.140625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="18" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="21" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" style="19" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" style="18" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="D1" s="27"/>
+    </row>
+    <row r="2" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
         <v>64</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="20" t="s">
         <v>52</v>
       </c>
       <c r="F2" s="11" t="s">
@@ -1131,246 +1309,246 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Add beta table sect 3
</commit_message>
<xml_diff>
--- a/Calcs/tables.xlsx
+++ b/Calcs/tables.xlsx
@@ -14,8 +14,9 @@
   <sheets>
     <sheet name="2.1" sheetId="1" r:id="rId1"/>
     <sheet name="2.2" sheetId="2" r:id="rId2"/>
-    <sheet name="4.1" sheetId="4" r:id="rId3"/>
-    <sheet name="5.1" sheetId="3" r:id="rId4"/>
+    <sheet name="3.1" sheetId="5" r:id="rId3"/>
+    <sheet name="4.1" sheetId="4" r:id="rId4"/>
+    <sheet name="5.1" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="108">
   <si>
     <t>$$</t>
   </si>
@@ -345,6 +346,12 @@
   </si>
   <si>
     <t>Simply supported ends, Capstan p z=0 various \mu</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>beta</t>
   </si>
 </sst>
 </file>
@@ -502,6 +509,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -512,9 +522,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -845,14 +852,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="24" t="s">
+      <c r="D1" s="26"/>
+      <c r="E1" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="24"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -1040,10 +1047,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="15"/>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="26"/>
+      <c r="C1" s="27"/>
       <c r="D1" s="14"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1145,9 +1152,115 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M16" sqref="L14:M16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
+        <v>0.125</v>
+      </c>
+      <c r="B2" s="12">
+        <f>(2.73/((14*A2)^2))^0.25</f>
+        <v>0.97167636122493573</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <f>A2+0.125</f>
+        <v>0.25</v>
+      </c>
+      <c r="B3" s="12">
+        <f t="shared" ref="B3:B9" si="0">(2.73/((14*A3)^2))^0.25</f>
+        <v>0.68707894414082138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <f t="shared" ref="A4:A9" si="1">A3+0.125</f>
+        <v>0.375</v>
+      </c>
+      <c r="B4" s="12">
+        <f t="shared" si="0"/>
+        <v>0.56099760871841264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="B5" s="12">
+        <f t="shared" si="0"/>
+        <v>0.48583818061246786</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <f t="shared" si="1"/>
+        <v>0.625</v>
+      </c>
+      <c r="B6" s="12">
+        <f t="shared" si="0"/>
+        <v>0.43454687916571944</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="B7" s="12">
+        <f t="shared" si="0"/>
+        <v>0.39668521335422707</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <f t="shared" si="1"/>
+        <v>0.875</v>
+      </c>
+      <c r="B8" s="12">
+        <f t="shared" si="0"/>
+        <v>0.36725914380590635</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="B9" s="12">
+        <f t="shared" si="0"/>
+        <v>0.34353947207041069</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1162,10 +1275,10 @@
       <c r="A1" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="24" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1263,7 +1376,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
@@ -1283,10 +1396,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="27"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">

</xml_diff>